<commit_message>
Se lleva el analiozador hasta mirory
</commit_message>
<xml_diff>
--- a/archivos/TOKENS.xlsx
+++ b/archivos/TOKENS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/737adc2e4267269d/Desktop/2do.Semestre2021/LENGUAJESFORMALES/Lab/Proyecto1/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B02E452-9EA0-49BC-A796-B79A32FFFDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{1B02E452-9EA0-49BC-A796-B79A32FFFDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA5503DD-7800-44DB-963C-7C2B2B19BCA5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E0686138-3DA5-4051-B5E6-54D93E449E57}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>Token</t>
   </si>
@@ -72,9 +72,6 @@
     <t>/;</t>
   </si>
   <si>
-    <t>entero_positivo</t>
-  </si>
-  <si>
     <t>secuencia de uno o más digitos</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>/,</t>
   </si>
   <si>
-    <t>parentesis</t>
-  </si>
-  <si>
     <t>Símbolo (</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>/)</t>
   </si>
   <si>
-    <t>Corchetes</t>
-  </si>
-  <si>
     <t>Símbolo [</t>
   </si>
   <si>
@@ -126,9 +117,6 @@
     <t>/]</t>
   </si>
   <si>
-    <t>Llaves</t>
-  </si>
-  <si>
     <t>Símbolo {</t>
   </si>
   <si>
@@ -144,9 +132,6 @@
     <t>Título</t>
   </si>
   <si>
-    <t>Secuencia de una o más palabras, digitos o simbolos encerrados en comillas</t>
-  </si>
-  <si>
     <t>Simbolo "</t>
   </si>
   <si>
@@ -156,9 +141,6 @@
     <t>/"</t>
   </si>
   <si>
-    <t>(comilla)(letra|simbolo|digito)(letra|simbolo|digito)*(comilla)</t>
-  </si>
-  <si>
     <t>Ancho</t>
   </si>
   <si>
@@ -168,9 +150,6 @@
     <t>{0..9}{0..9}*</t>
   </si>
   <si>
-    <t>(digito)(digito)*</t>
-  </si>
-  <si>
     <t>Alto</t>
   </si>
   <si>
@@ -183,9 +162,6 @@
     <t>Celdas</t>
   </si>
   <si>
-    <t>Llave izquierda Secuencia de: (corchete derecho, entero positivo, coma,entero positivo, coma, booleano, coma, color, corchete derecho, coma, salto de línea)</t>
-  </si>
-  <si>
     <t>Número</t>
   </si>
   <si>
@@ -198,9 +174,6 @@
     <t>#(Letrahex|digito)(Letrahex|digito)(Letrahex|digito)(Letrahex|digito)(Letrahex|digito)(Letrahex|digito)</t>
   </si>
   <si>
-    <t>{ ([entero_positivo,entero_positivo,(True|False),Color_hex],)*  ([entero_positivo,entero_positivo,(True|False),Color_hex])};</t>
-  </si>
-  <si>
     <t>Filtros</t>
   </si>
   <si>
@@ -213,10 +186,64 @@
     <t>Seperadorde imágenes</t>
   </si>
   <si>
-    <t xml:space="preserve">Palabra MIRRORX, MIRRORY O DOUBLEMIRROR PUEDEN SER LAS 3 O NINGUNA </t>
-  </si>
-  <si>
-    <t>(MIRRORX,|MIRRORY,|DOUBLEMIRROR)* (MIRRORX|MIRRORY|DOUBLEMIRROR);*</t>
+    <t>parentesis izquierdo</t>
+  </si>
+  <si>
+    <t>parentesis derecho</t>
+  </si>
+  <si>
+    <t>Corchete izquierdo</t>
+  </si>
+  <si>
+    <t>Llave derecha</t>
+  </si>
+  <si>
+    <t>Llave izquierda</t>
+  </si>
+  <si>
+    <t>Corchete derecho</t>
+  </si>
+  <si>
+    <t>TITULO</t>
+  </si>
+  <si>
+    <t>ANCHO</t>
+  </si>
+  <si>
+    <t>ALTO</t>
+  </si>
+  <si>
+    <t>FILAS</t>
+  </si>
+  <si>
+    <t>COLUMNAS</t>
+  </si>
+  <si>
+    <t>CELDAS</t>
+  </si>
+  <si>
+    <t>FILTROS</t>
+  </si>
+  <si>
+    <t>MIRRORX</t>
+  </si>
+  <si>
+    <t>MIRRORY</t>
+  </si>
+  <si>
+    <t>DOUBLEMIRROR</t>
+  </si>
+  <si>
+    <t>SIMBOLO</t>
+  </si>
+  <si>
+    <t>CUALQUIER SIMBOLO</t>
+  </si>
+  <si>
+    <t>/(SIMBOLO)+</t>
+  </si>
+  <si>
+    <t>enteropositivo</t>
   </si>
 </sst>
 </file>
@@ -695,15 +722,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1EAF14-7125-449F-BE4C-75DE3F75CC4F}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.109375" customWidth="1"/>
   </cols>
@@ -732,13 +759,13 @@
     </row>
     <row r="3" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -763,211 +790,255 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="12" t="s">
+      <c r="B18" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="B19" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>47</v>
-      </c>
       <c r="B20" s="8" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="249.6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="109.2" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>57</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>